<commit_message>
feat: adicionando redução de dimensionalidade
</commit_message>
<xml_diff>
--- a/cluster_normalizado.xlsx
+++ b/cluster_normalizado.xlsx
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -864,7 +864,7 @@
         <v>0.5</v>
       </c>
       <c r="AA5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1030,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="AA7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="AA9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1362,7 +1362,7 @@
         <v>0.5</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -1445,7 +1445,7 @@
         <v>0.5</v>
       </c>
       <c r="AA12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -1528,7 +1528,7 @@
         <v>0.5</v>
       </c>
       <c r="AA13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -1611,7 +1611,7 @@
         <v>0.5</v>
       </c>
       <c r="AA14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="AA19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -2109,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="AA20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -2192,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="AA21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -2275,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="AA22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -2358,7 +2358,7 @@
         <v>0.5</v>
       </c>
       <c r="AA23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -2441,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="AA24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -2524,7 +2524,7 @@
         <v>0.5</v>
       </c>
       <c r="AA25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="AA26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -2690,7 +2690,7 @@
         <v>0.5</v>
       </c>
       <c r="AA27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="AA28">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -2939,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="AA30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -3022,7 +3022,7 @@
         <v>0.5</v>
       </c>
       <c r="AA31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -3105,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="AA32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:27">
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="AA34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:27">
@@ -3354,7 +3354,7 @@
         <v>0.5</v>
       </c>
       <c r="AA35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:27">
@@ -3437,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="AA36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:27">
@@ -3520,7 +3520,7 @@
         <v>0.5</v>
       </c>
       <c r="AA37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:27">
@@ -3769,7 +3769,7 @@
         <v>1</v>
       </c>
       <c r="AA40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:27">
@@ -3852,7 +3852,7 @@
         <v>0.5</v>
       </c>
       <c r="AA41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:27">
@@ -3935,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="AA42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:27">
@@ -4018,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="AA43">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:27">
@@ -4101,7 +4101,7 @@
         <v>0.5</v>
       </c>
       <c r="AA44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:27">
@@ -4184,7 +4184,7 @@
         <v>0</v>
       </c>
       <c r="AA45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:27">
@@ -4267,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="AA46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:27">
@@ -4350,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="AA47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:27">
@@ -4433,7 +4433,7 @@
         <v>0.5</v>
       </c>
       <c r="AA48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:27">
@@ -4516,7 +4516,7 @@
         <v>0.5</v>
       </c>
       <c r="AA49">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:27">
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="AA50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:27">
@@ -4765,7 +4765,7 @@
         <v>0.5</v>
       </c>
       <c r="AA52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:27">
@@ -4848,7 +4848,7 @@
         <v>0.5</v>
       </c>
       <c r="AA53">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:27">
@@ -4931,7 +4931,7 @@
         <v>0.5</v>
       </c>
       <c r="AA54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:27">
@@ -5014,7 +5014,7 @@
         <v>0.5</v>
       </c>
       <c r="AA55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:27">
@@ -5097,7 +5097,7 @@
         <v>0</v>
       </c>
       <c r="AA56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:27">
@@ -5263,7 +5263,7 @@
         <v>0</v>
       </c>
       <c r="AA58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:27">
@@ -5346,7 +5346,7 @@
         <v>0.5</v>
       </c>
       <c r="AA59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:27">
@@ -5429,7 +5429,7 @@
         <v>0.5</v>
       </c>
       <c r="AA60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:27">
@@ -5512,7 +5512,7 @@
         <v>0.5</v>
       </c>
       <c r="AA61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:27">
@@ -5595,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="AA62">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:27">
@@ -5678,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="AA63">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:27">
@@ -5761,7 +5761,7 @@
         <v>0.5</v>
       </c>
       <c r="AA64">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:27">
@@ -5844,7 +5844,7 @@
         <v>1</v>
       </c>
       <c r="AA65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:27">
@@ -6010,7 +6010,7 @@
         <v>0</v>
       </c>
       <c r="AA67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:27">
@@ -6093,7 +6093,7 @@
         <v>0.5</v>
       </c>
       <c r="AA68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:27">
@@ -6176,7 +6176,7 @@
         <v>1</v>
       </c>
       <c r="AA69">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:27">
@@ -6259,7 +6259,7 @@
         <v>1</v>
       </c>
       <c r="AA70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:27">
@@ -6425,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="AA72">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:27">
@@ -6508,7 +6508,7 @@
         <v>1</v>
       </c>
       <c r="AA73">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:27">
@@ -6591,7 +6591,7 @@
         <v>0.5</v>
       </c>
       <c r="AA74">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:27">
@@ -6674,7 +6674,7 @@
         <v>0.5</v>
       </c>
       <c r="AA75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:27">
@@ -6840,7 +6840,7 @@
         <v>0.5</v>
       </c>
       <c r="AA77">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:27">
@@ -6923,7 +6923,7 @@
         <v>1</v>
       </c>
       <c r="AA78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:27">
@@ -7006,7 +7006,7 @@
         <v>0</v>
       </c>
       <c r="AA79">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:27">
@@ -7089,7 +7089,7 @@
         <v>0</v>
       </c>
       <c r="AA80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:27">
@@ -7172,7 +7172,7 @@
         <v>0.5</v>
       </c>
       <c r="AA81">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:27">
@@ -7255,7 +7255,7 @@
         <v>1</v>
       </c>
       <c r="AA82">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:27">
@@ -7338,7 +7338,7 @@
         <v>1</v>
       </c>
       <c r="AA83">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:27">
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="AA85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:27">
@@ -7587,7 +7587,7 @@
         <v>0.5</v>
       </c>
       <c r="AA86">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:27">
@@ -7670,7 +7670,7 @@
         <v>0.5</v>
       </c>
       <c r="AA87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:27">
@@ -7753,7 +7753,7 @@
         <v>1</v>
       </c>
       <c r="AA88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:27">
@@ -7836,7 +7836,7 @@
         <v>0.5</v>
       </c>
       <c r="AA89">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:27">
@@ -7919,7 +7919,7 @@
         <v>0.5</v>
       </c>
       <c r="AA90">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:27">
@@ -8251,7 +8251,7 @@
         <v>0.5</v>
       </c>
       <c r="AA94">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:27">
@@ -8417,7 +8417,7 @@
         <v>0.5</v>
       </c>
       <c r="AA96">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:27">
@@ -8583,7 +8583,7 @@
         <v>0.5</v>
       </c>
       <c r="AA98">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:27">
@@ -8666,7 +8666,7 @@
         <v>1</v>
       </c>
       <c r="AA99">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:27">
@@ -8749,7 +8749,7 @@
         <v>1</v>
       </c>
       <c r="AA100">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:27">
@@ -8832,7 +8832,7 @@
         <v>0.5</v>
       </c>
       <c r="AA101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:27">
@@ -8915,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="AA102">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:27">
@@ -8998,7 +8998,7 @@
         <v>0.5</v>
       </c>
       <c r="AA103">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:27">
@@ -9247,7 +9247,7 @@
         <v>0.5</v>
       </c>
       <c r="AA106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:27">
@@ -9330,7 +9330,7 @@
         <v>0.5</v>
       </c>
       <c r="AA107">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:27">
@@ -9413,7 +9413,7 @@
         <v>0.5</v>
       </c>
       <c r="AA108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:27">
@@ -9579,7 +9579,7 @@
         <v>1</v>
       </c>
       <c r="AA110">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:27">
@@ -9745,7 +9745,7 @@
         <v>0</v>
       </c>
       <c r="AA112">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:27">
@@ -9828,7 +9828,7 @@
         <v>0.5</v>
       </c>
       <c r="AA113">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:27">
@@ -9994,7 +9994,7 @@
         <v>0.5</v>
       </c>
       <c r="AA115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:27">
@@ -10077,7 +10077,7 @@
         <v>0</v>
       </c>
       <c r="AA116">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:27">
@@ -10160,7 +10160,7 @@
         <v>0.5</v>
       </c>
       <c r="AA117">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:27">
@@ -10243,7 +10243,7 @@
         <v>0.5</v>
       </c>
       <c r="AA118">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:27">
@@ -10326,7 +10326,7 @@
         <v>0.5</v>
       </c>
       <c r="AA119">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:27">
@@ -10409,7 +10409,7 @@
         <v>0</v>
       </c>
       <c r="AA120">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:27">
@@ -10492,7 +10492,7 @@
         <v>0.5</v>
       </c>
       <c r="AA121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:27">
@@ -10575,7 +10575,7 @@
         <v>0</v>
       </c>
       <c r="AA122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:27">
@@ -10658,7 +10658,7 @@
         <v>0</v>
       </c>
       <c r="AA123">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:27">
@@ -10824,7 +10824,7 @@
         <v>1</v>
       </c>
       <c r="AA125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:27">
@@ -10907,7 +10907,7 @@
         <v>0.5</v>
       </c>
       <c r="AA126">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:27">
@@ -10990,7 +10990,7 @@
         <v>0</v>
       </c>
       <c r="AA127">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:27">
@@ -11073,7 +11073,7 @@
         <v>0.5</v>
       </c>
       <c r="AA128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:27">
@@ -11156,7 +11156,7 @@
         <v>0.5</v>
       </c>
       <c r="AA129">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:27">
@@ -11239,7 +11239,7 @@
         <v>1</v>
       </c>
       <c r="AA130">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:27">
@@ -11322,7 +11322,7 @@
         <v>0.5</v>
       </c>
       <c r="AA131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:27">
@@ -11488,7 +11488,7 @@
         <v>0.5</v>
       </c>
       <c r="AA133">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:27">
@@ -11571,7 +11571,7 @@
         <v>0.5</v>
       </c>
       <c r="AA134">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:27">
@@ -11654,7 +11654,7 @@
         <v>0.5</v>
       </c>
       <c r="AA135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:27">
@@ -11737,7 +11737,7 @@
         <v>1</v>
       </c>
       <c r="AA136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:27">
@@ -11986,7 +11986,7 @@
         <v>0.5</v>
       </c>
       <c r="AA139">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:27">
@@ -12069,7 +12069,7 @@
         <v>1</v>
       </c>
       <c r="AA140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:27">
@@ -12152,7 +12152,7 @@
         <v>0</v>
       </c>
       <c r="AA141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:27">
@@ -12235,7 +12235,7 @@
         <v>0</v>
       </c>
       <c r="AA142">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:27">
@@ -12401,7 +12401,7 @@
         <v>0.5</v>
       </c>
       <c r="AA144">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:27">
@@ -12484,7 +12484,7 @@
         <v>1</v>
       </c>
       <c r="AA145">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:27">
@@ -12567,7 +12567,7 @@
         <v>0</v>
       </c>
       <c r="AA146">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:27">
@@ -12650,7 +12650,7 @@
         <v>0.5</v>
       </c>
       <c r="AA147">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:27">
@@ -12733,7 +12733,7 @@
         <v>1</v>
       </c>
       <c r="AA148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:27">
@@ -12816,7 +12816,7 @@
         <v>1</v>
       </c>
       <c r="AA149">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:27">
@@ -12899,7 +12899,7 @@
         <v>0.5</v>
       </c>
       <c r="AA150">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:27">
@@ -12982,7 +12982,7 @@
         <v>1</v>
       </c>
       <c r="AA151">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:27">
@@ -13065,7 +13065,7 @@
         <v>0</v>
       </c>
       <c r="AA152">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:27">
@@ -13148,7 +13148,7 @@
         <v>0</v>
       </c>
       <c r="AA153">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:27">
@@ -13231,7 +13231,7 @@
         <v>0</v>
       </c>
       <c r="AA154">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:27">
@@ -13314,7 +13314,7 @@
         <v>0</v>
       </c>
       <c r="AA155">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:27">
@@ -13480,7 +13480,7 @@
         <v>0</v>
       </c>
       <c r="AA157">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:27">
@@ -13729,7 +13729,7 @@
         <v>1</v>
       </c>
       <c r="AA160">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clusters nor e naonorm
</commit_message>
<xml_diff>
--- a/cluster_normalizado.xlsx
+++ b/cluster_normalizado.xlsx
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -864,7 +864,7 @@
         <v>0.5</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -1030,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="AA7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="AA8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1445,7 +1445,7 @@
         <v>0.5</v>
       </c>
       <c r="AA12">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -1528,7 +1528,7 @@
         <v>0.5</v>
       </c>
       <c r="AA13">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:27">
@@ -1611,7 +1611,7 @@
         <v>0.5</v>
       </c>
       <c r="AA14">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:27">
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -1943,7 +1943,7 @@
         <v>0.5</v>
       </c>
       <c r="AA18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="AA19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -2109,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="AA20">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -2192,7 +2192,7 @@
         <v>1</v>
       </c>
       <c r="AA21">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -2275,7 +2275,7 @@
         <v>0</v>
       </c>
       <c r="AA22">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -2358,7 +2358,7 @@
         <v>0.5</v>
       </c>
       <c r="AA23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:27">
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="AA28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="AA29">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -3105,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="AA32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:27">
@@ -3188,7 +3188,7 @@
         <v>0.5</v>
       </c>
       <c r="AA33">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:27">
@@ -3354,7 +3354,7 @@
         <v>0.5</v>
       </c>
       <c r="AA35">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:27">
@@ -3437,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="AA36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:27">
@@ -3603,7 +3603,7 @@
         <v>0.5</v>
       </c>
       <c r="AA38">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:27">
@@ -3686,7 +3686,7 @@
         <v>1</v>
       </c>
       <c r="AA39">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:27">
@@ -3769,7 +3769,7 @@
         <v>1</v>
       </c>
       <c r="AA40">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:27">
@@ -3935,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="AA42">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:27">
@@ -4018,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="AA43">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:27">
@@ -4101,7 +4101,7 @@
         <v>0.5</v>
       </c>
       <c r="AA44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:27">
@@ -4267,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="AA46">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:27">
@@ -4433,7 +4433,7 @@
         <v>0.5</v>
       </c>
       <c r="AA48">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:27">
@@ -4516,7 +4516,7 @@
         <v>0.5</v>
       </c>
       <c r="AA49">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:27">
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="AA50">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:27">
@@ -4682,7 +4682,7 @@
         <v>0.5</v>
       </c>
       <c r="AA51">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:27">
@@ -4848,7 +4848,7 @@
         <v>0.5</v>
       </c>
       <c r="AA53">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:27">
@@ -4931,7 +4931,7 @@
         <v>0.5</v>
       </c>
       <c r="AA54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:27">
@@ -5014,7 +5014,7 @@
         <v>0.5</v>
       </c>
       <c r="AA55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:27">
@@ -5097,7 +5097,7 @@
         <v>0</v>
       </c>
       <c r="AA56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:27">
@@ -5180,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="AA57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:27">
@@ -5678,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="AA63">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:27">
@@ -5761,7 +5761,7 @@
         <v>0.5</v>
       </c>
       <c r="AA64">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:27">
@@ -5927,7 +5927,7 @@
         <v>0.5</v>
       </c>
       <c r="AA66">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:27">
@@ -6010,7 +6010,7 @@
         <v>0</v>
       </c>
       <c r="AA67">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:27">
@@ -6176,7 +6176,7 @@
         <v>1</v>
       </c>
       <c r="AA69">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:27">
@@ -6259,7 +6259,7 @@
         <v>1</v>
       </c>
       <c r="AA70">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:27">
@@ -6342,7 +6342,7 @@
         <v>0</v>
       </c>
       <c r="AA71">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:27">
@@ -6425,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="AA72">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:27">
@@ -6508,7 +6508,7 @@
         <v>1</v>
       </c>
       <c r="AA73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:27">
@@ -6757,7 +6757,7 @@
         <v>1</v>
       </c>
       <c r="AA76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:27">
@@ -6840,7 +6840,7 @@
         <v>0.5</v>
       </c>
       <c r="AA77">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:27">
@@ -7006,7 +7006,7 @@
         <v>0</v>
       </c>
       <c r="AA79">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:27">
@@ -7089,7 +7089,7 @@
         <v>0</v>
       </c>
       <c r="AA80">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:27">
@@ -7255,7 +7255,7 @@
         <v>1</v>
       </c>
       <c r="AA82">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:27">
@@ -7338,7 +7338,7 @@
         <v>1</v>
       </c>
       <c r="AA83">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:27">
@@ -7421,7 +7421,7 @@
         <v>0.5</v>
       </c>
       <c r="AA84">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:27">
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="AA85">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:27">
@@ -7753,7 +7753,7 @@
         <v>1</v>
       </c>
       <c r="AA88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:27">
@@ -7836,7 +7836,7 @@
         <v>0.5</v>
       </c>
       <c r="AA89">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:27">
@@ -7919,7 +7919,7 @@
         <v>0.5</v>
       </c>
       <c r="AA90">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:27">
@@ -8002,7 +8002,7 @@
         <v>0.5</v>
       </c>
       <c r="AA91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:27">
@@ -8085,7 +8085,7 @@
         <v>0.5</v>
       </c>
       <c r="AA92">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:27">
@@ -8168,7 +8168,7 @@
         <v>0</v>
       </c>
       <c r="AA93">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:27">
@@ -8334,7 +8334,7 @@
         <v>0.5</v>
       </c>
       <c r="AA95">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:27">
@@ -8500,7 +8500,7 @@
         <v>1</v>
       </c>
       <c r="AA97">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:27">
@@ -8583,7 +8583,7 @@
         <v>0.5</v>
       </c>
       <c r="AA98">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:27">
@@ -8666,7 +8666,7 @@
         <v>1</v>
       </c>
       <c r="AA99">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:27">
@@ -8915,7 +8915,7 @@
         <v>0</v>
       </c>
       <c r="AA102">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:27">
@@ -9081,7 +9081,7 @@
         <v>1</v>
       </c>
       <c r="AA104">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:27">
@@ -9164,7 +9164,7 @@
         <v>1</v>
       </c>
       <c r="AA105">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:27">
@@ -9496,7 +9496,7 @@
         <v>0.5</v>
       </c>
       <c r="AA109">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:27">
@@ -9579,7 +9579,7 @@
         <v>1</v>
       </c>
       <c r="AA110">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:27">
@@ -9662,7 +9662,7 @@
         <v>0.5</v>
       </c>
       <c r="AA111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:27">
@@ -9745,7 +9745,7 @@
         <v>0</v>
       </c>
       <c r="AA112">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:27">
@@ -9828,7 +9828,7 @@
         <v>0.5</v>
       </c>
       <c r="AA113">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:27">
@@ -9911,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="AA114">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:27">
@@ -10326,7 +10326,7 @@
         <v>0.5</v>
       </c>
       <c r="AA119">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:27">
@@ -10658,7 +10658,7 @@
         <v>0</v>
       </c>
       <c r="AA123">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:27">
@@ -10741,7 +10741,7 @@
         <v>0.5</v>
       </c>
       <c r="AA124">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:27">
@@ -10907,7 +10907,7 @@
         <v>0.5</v>
       </c>
       <c r="AA126">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:27">
@@ -10990,7 +10990,7 @@
         <v>0</v>
       </c>
       <c r="AA127">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:27">
@@ -11073,7 +11073,7 @@
         <v>0.5</v>
       </c>
       <c r="AA128">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:27">
@@ -11156,7 +11156,7 @@
         <v>0.5</v>
       </c>
       <c r="AA129">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:27">
@@ -11239,7 +11239,7 @@
         <v>1</v>
       </c>
       <c r="AA130">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:27">
@@ -11405,7 +11405,7 @@
         <v>1</v>
       </c>
       <c r="AA132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:27">
@@ -11488,7 +11488,7 @@
         <v>0.5</v>
       </c>
       <c r="AA133">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:27">
@@ -11571,7 +11571,7 @@
         <v>0.5</v>
       </c>
       <c r="AA134">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:27">
@@ -11820,7 +11820,7 @@
         <v>0.5</v>
       </c>
       <c r="AA137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:27">
@@ -11903,7 +11903,7 @@
         <v>0.5</v>
       </c>
       <c r="AA138">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:27">
@@ -11986,7 +11986,7 @@
         <v>0.5</v>
       </c>
       <c r="AA139">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:27">
@@ -12069,7 +12069,7 @@
         <v>1</v>
       </c>
       <c r="AA140">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:27">
@@ -12152,7 +12152,7 @@
         <v>0</v>
       </c>
       <c r="AA141">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:27">
@@ -12235,7 +12235,7 @@
         <v>0</v>
       </c>
       <c r="AA142">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:27">
@@ -12318,7 +12318,7 @@
         <v>0.5</v>
       </c>
       <c r="AA143">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:27">
@@ -12484,7 +12484,7 @@
         <v>1</v>
       </c>
       <c r="AA145">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:27">
@@ -12650,7 +12650,7 @@
         <v>0.5</v>
       </c>
       <c r="AA147">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:27">
@@ -12816,7 +12816,7 @@
         <v>1</v>
       </c>
       <c r="AA149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:27">
@@ -12899,7 +12899,7 @@
         <v>0.5</v>
       </c>
       <c r="AA150">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:27">
@@ -12982,7 +12982,7 @@
         <v>1</v>
       </c>
       <c r="AA151">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:27">
@@ -13065,7 +13065,7 @@
         <v>0</v>
       </c>
       <c r="AA152">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:27">
@@ -13148,7 +13148,7 @@
         <v>0</v>
       </c>
       <c r="AA153">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:27">
@@ -13314,7 +13314,7 @@
         <v>0</v>
       </c>
       <c r="AA155">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:27">
@@ -13397,7 +13397,7 @@
         <v>0</v>
       </c>
       <c r="AA156">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:27">
@@ -13563,7 +13563,7 @@
         <v>0.5</v>
       </c>
       <c r="AA158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:27">
@@ -13646,7 +13646,7 @@
         <v>1</v>
       </c>
       <c r="AA159">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:27">
@@ -13729,7 +13729,7 @@
         <v>1</v>
       </c>
       <c r="AA160">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: adicionando cluster na base original
</commit_message>
<xml_diff>
--- a/cluster_normalizado.xlsx
+++ b/cluster_normalizado.xlsx
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="AA2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -864,7 +864,7 @@
         <v>0.5</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27">
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="AA6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
       <c r="AA9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="AA10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -1362,7 +1362,7 @@
         <v>0.5</v>
       </c>
       <c r="AA11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:27">
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:27">
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -1943,7 +1943,7 @@
         <v>0.5</v>
       </c>
       <c r="AA18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
       <c r="AA19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -2441,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="AA24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -2524,7 +2524,7 @@
         <v>0.5</v>
       </c>
       <c r="AA25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:27">
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="AA26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:27">
@@ -2690,7 +2690,7 @@
         <v>0.5</v>
       </c>
       <c r="AA27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -2773,7 +2773,7 @@
         <v>1</v>
       </c>
       <c r="AA28">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="AA29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -2939,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="AA30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:27">
@@ -3022,7 +3022,7 @@
         <v>0.5</v>
       </c>
       <c r="AA31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -3105,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="AA32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:27">
@@ -3188,7 +3188,7 @@
         <v>0.5</v>
       </c>
       <c r="AA33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:27">
@@ -3271,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="AA34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:27">
@@ -3354,7 +3354,7 @@
         <v>0.5</v>
       </c>
       <c r="AA35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:27">
@@ -3437,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="AA36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:27">
@@ -3520,7 +3520,7 @@
         <v>0.5</v>
       </c>
       <c r="AA37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:27">
@@ -3603,7 +3603,7 @@
         <v>0.5</v>
       </c>
       <c r="AA38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:27">
@@ -3686,7 +3686,7 @@
         <v>1</v>
       </c>
       <c r="AA39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:27">
@@ -4101,7 +4101,7 @@
         <v>0.5</v>
       </c>
       <c r="AA44">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:27">
@@ -4184,7 +4184,7 @@
         <v>0</v>
       </c>
       <c r="AA45">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:27">
@@ -4350,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="AA47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:27">
@@ -4682,7 +4682,7 @@
         <v>0.5</v>
       </c>
       <c r="AA51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:27">
@@ -4765,7 +4765,7 @@
         <v>0.5</v>
       </c>
       <c r="AA52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:27">
@@ -4931,7 +4931,7 @@
         <v>0.5</v>
       </c>
       <c r="AA54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:27">
@@ -5014,7 +5014,7 @@
         <v>0.5</v>
       </c>
       <c r="AA55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:27">
@@ -5263,7 +5263,7 @@
         <v>0</v>
       </c>
       <c r="AA58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:27">
@@ -5346,7 +5346,7 @@
         <v>0.5</v>
       </c>
       <c r="AA59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:27">
@@ -5512,7 +5512,7 @@
         <v>0.5</v>
       </c>
       <c r="AA61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:27">
@@ -5595,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="AA62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:27">
@@ -5678,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="AA63">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:27">
@@ -5844,7 +5844,7 @@
         <v>1</v>
       </c>
       <c r="AA65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:27">
@@ -5927,7 +5927,7 @@
         <v>0.5</v>
       </c>
       <c r="AA66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:27">
@@ -6093,7 +6093,7 @@
         <v>0.5</v>
       </c>
       <c r="AA68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:27">
@@ -6176,7 +6176,7 @@
         <v>1</v>
       </c>
       <c r="AA69">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:27">
@@ -6259,7 +6259,7 @@
         <v>1</v>
       </c>
       <c r="AA70">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:27">
@@ -6342,7 +6342,7 @@
         <v>0</v>
       </c>
       <c r="AA71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:27">
@@ -6425,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="AA72">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:27">
@@ -6508,7 +6508,7 @@
         <v>1</v>
       </c>
       <c r="AA73">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:27">
@@ -6591,7 +6591,7 @@
         <v>0.5</v>
       </c>
       <c r="AA74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:27">
@@ -6674,7 +6674,7 @@
         <v>0.5</v>
       </c>
       <c r="AA75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:27">
@@ -6840,7 +6840,7 @@
         <v>0.5</v>
       </c>
       <c r="AA77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:27">
@@ -6923,7 +6923,7 @@
         <v>1</v>
       </c>
       <c r="AA78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:27">
@@ -7089,7 +7089,7 @@
         <v>0</v>
       </c>
       <c r="AA80">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:27">
@@ -7172,7 +7172,7 @@
         <v>0.5</v>
       </c>
       <c r="AA81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:27">
@@ -7255,7 +7255,7 @@
         <v>1</v>
       </c>
       <c r="AA82">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:27">
@@ -7421,7 +7421,7 @@
         <v>0.5</v>
       </c>
       <c r="AA84">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:27">
@@ -7504,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="AA85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:27">
@@ -7587,7 +7587,7 @@
         <v>0.5</v>
       </c>
       <c r="AA86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:27">
@@ -7670,7 +7670,7 @@
         <v>0.5</v>
       </c>
       <c r="AA87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:27">
@@ -7753,7 +7753,7 @@
         <v>1</v>
       </c>
       <c r="AA88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:27">
@@ -7919,7 +7919,7 @@
         <v>0.5</v>
       </c>
       <c r="AA90">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:27">
@@ -8085,7 +8085,7 @@
         <v>0.5</v>
       </c>
       <c r="AA92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:27">
@@ -8168,7 +8168,7 @@
         <v>0</v>
       </c>
       <c r="AA93">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:27">
@@ -8251,7 +8251,7 @@
         <v>0.5</v>
       </c>
       <c r="AA94">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:27">
@@ -8334,7 +8334,7 @@
         <v>0.5</v>
       </c>
       <c r="AA95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:27">
@@ -8417,7 +8417,7 @@
         <v>0.5</v>
       </c>
       <c r="AA96">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:27">
@@ -8666,7 +8666,7 @@
         <v>1</v>
       </c>
       <c r="AA99">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:27">
@@ -8749,7 +8749,7 @@
         <v>1</v>
       </c>
       <c r="AA100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:27">
@@ -8832,7 +8832,7 @@
         <v>0.5</v>
       </c>
       <c r="AA101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:27">
@@ -8998,7 +8998,7 @@
         <v>0.5</v>
       </c>
       <c r="AA103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:27">
@@ -9081,7 +9081,7 @@
         <v>1</v>
       </c>
       <c r="AA104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:27">
@@ -9247,7 +9247,7 @@
         <v>0.5</v>
       </c>
       <c r="AA106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:27">
@@ -9330,7 +9330,7 @@
         <v>0.5</v>
       </c>
       <c r="AA107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:27">
@@ -9413,7 +9413,7 @@
         <v>0.5</v>
       </c>
       <c r="AA108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:27">
@@ -9496,7 +9496,7 @@
         <v>0.5</v>
       </c>
       <c r="AA109">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:27">
@@ -9579,7 +9579,7 @@
         <v>1</v>
       </c>
       <c r="AA110">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:27">
@@ -9911,7 +9911,7 @@
         <v>1</v>
       </c>
       <c r="AA114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:27">
@@ -9994,7 +9994,7 @@
         <v>0.5</v>
       </c>
       <c r="AA115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:27">
@@ -10077,7 +10077,7 @@
         <v>0</v>
       </c>
       <c r="AA116">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:27">
@@ -10160,7 +10160,7 @@
         <v>0.5</v>
       </c>
       <c r="AA117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:27">
@@ -10243,7 +10243,7 @@
         <v>0.5</v>
       </c>
       <c r="AA118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:27">
@@ -10326,7 +10326,7 @@
         <v>0.5</v>
       </c>
       <c r="AA119">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:27">
@@ -10409,7 +10409,7 @@
         <v>0</v>
       </c>
       <c r="AA120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:27">
@@ -10492,7 +10492,7 @@
         <v>0.5</v>
       </c>
       <c r="AA121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:27">
@@ -10575,7 +10575,7 @@
         <v>0</v>
       </c>
       <c r="AA122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:27">
@@ -10658,7 +10658,7 @@
         <v>0</v>
       </c>
       <c r="AA123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:27">
@@ -10741,7 +10741,7 @@
         <v>0.5</v>
       </c>
       <c r="AA124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:27">
@@ -10824,7 +10824,7 @@
         <v>1</v>
       </c>
       <c r="AA125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:27">
@@ -11239,7 +11239,7 @@
         <v>1</v>
       </c>
       <c r="AA130">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:27">
@@ -11322,7 +11322,7 @@
         <v>0.5</v>
       </c>
       <c r="AA131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:27">
@@ -11488,7 +11488,7 @@
         <v>0.5</v>
       </c>
       <c r="AA133">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:27">
@@ -11571,7 +11571,7 @@
         <v>0.5</v>
       </c>
       <c r="AA134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:27">
@@ -11654,7 +11654,7 @@
         <v>0.5</v>
       </c>
       <c r="AA135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:27">
@@ -11737,7 +11737,7 @@
         <v>1</v>
       </c>
       <c r="AA136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:27">
@@ -11903,7 +11903,7 @@
         <v>0.5</v>
       </c>
       <c r="AA138">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:27">
@@ -12069,7 +12069,7 @@
         <v>1</v>
       </c>
       <c r="AA140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:27">
@@ -12152,7 +12152,7 @@
         <v>0</v>
       </c>
       <c r="AA141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:27">
@@ -12318,7 +12318,7 @@
         <v>0.5</v>
       </c>
       <c r="AA143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:27">
@@ -12401,7 +12401,7 @@
         <v>0.5</v>
       </c>
       <c r="AA144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:27">
@@ -12484,7 +12484,7 @@
         <v>1</v>
       </c>
       <c r="AA145">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:27">
@@ -12567,7 +12567,7 @@
         <v>0</v>
       </c>
       <c r="AA146">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:27">
@@ -12650,7 +12650,7 @@
         <v>0.5</v>
       </c>
       <c r="AA147">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:27">
@@ -12733,7 +12733,7 @@
         <v>1</v>
       </c>
       <c r="AA148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:27">
@@ -12899,7 +12899,7 @@
         <v>0.5</v>
       </c>
       <c r="AA150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:27">
@@ -12982,7 +12982,7 @@
         <v>1</v>
       </c>
       <c r="AA151">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:27">
@@ -13148,7 +13148,7 @@
         <v>0</v>
       </c>
       <c r="AA153">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:27">
@@ -13231,7 +13231,7 @@
         <v>0</v>
       </c>
       <c r="AA154">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:27">
@@ -13314,7 +13314,7 @@
         <v>0</v>
       </c>
       <c r="AA155">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:27">
@@ -13397,7 +13397,7 @@
         <v>0</v>
       </c>
       <c r="AA156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:27">
@@ -13480,7 +13480,7 @@
         <v>0</v>
       </c>
       <c r="AA157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:27">
@@ -13646,7 +13646,7 @@
         <v>1</v>
       </c>
       <c r="AA159">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:27">
@@ -13729,7 +13729,7 @@
         <v>1</v>
       </c>
       <c r="AA160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>